<commit_message>
petri nets para 20 casos
</commit_message>
<xml_diff>
--- a/src/atom/Csv/New/normales/sample_data.xlsx
+++ b/src/atom/Csv/New/normales/sample_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,31 +448,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FitAnormal_robot18_pros.csv</t>
+          <t>FitA_perefect</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{0.32500000000000007}</t>
+          <t>{0.42499999999999993}</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FitAnormal_robot3_pros.csv</t>
+          <t>FitAnormal_robot18_pros.csv</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{0.42499999999999993}</t>
+          <t>{0.32500000000000007}</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FitAnormal_robot9_pros.csv</t>
+          <t>FitAnormal_robot3_pros.csv</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,43 +484,43 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FitAnormal_robot19_pros.csv</t>
+          <t>FitAnormal_robot9_pros.csv</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>{0.32500000000000007}</t>
+          <t>{0.42499999999999993}</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FitAnormal_robot12_pros.csv</t>
+          <t>FitAnormal_robot19_pros.csv</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{0.375}</t>
+          <t>{0.32500000000000007}</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FitAnormal_robot1_pros.csv</t>
+          <t>FitAnormal_robot12_pros.csv</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{0.42499999999999993}</t>
+          <t>{0.375}</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>FitAnormal_robot6_pros.csv</t>
+          <t>FitAnormal_robot1_pros.csv</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FitAnormal_robot2_pros.csv</t>
+          <t>FitAnormal_robot6_pros.csv</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,142 +544,154 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>FitAnormal_robot11_pros.csv</t>
+          <t>FitAnormal_robot2_pros.csv</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>{0.375}</t>
+          <t>{0.42499999999999993}</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>FitAnormal_robot4_pros.csv</t>
+          <t>FitAnormal_robot11_pros.csv</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>{0.42499999999999993}</t>
+          <t>{0.375}</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>FitAnormal_robot20_pros.csv</t>
+          <t>FitAnormal_robot4_pros.csv</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>{0.32500000000000007}</t>
+          <t>{0.42499999999999993}</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>FitAnormal_robot10_pros.csv</t>
+          <t>FitAnormal_robot20_pros.csv</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>{0.42499999999999993}</t>
+          <t>{0.32500000000000007}</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>FitAnormal_robot14_pros.csv</t>
+          <t>FitAnormal_robot10_pros.csv</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>{0.375}</t>
+          <t>{0.42499999999999993}</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>FitAnormal_robot8_pros.csv</t>
+          <t>FitAnormal_robot14_pros.csv</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>{0.42499999999999993}</t>
+          <t>{0.375}</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>FitAnormal_robot16_pros.csv</t>
+          <t>FitAnormal_robot8_pros.csv</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>{0.32500000000000007}</t>
+          <t>{0.42499999999999993}</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>FitAnormal_robot7_pros.csv</t>
+          <t>FitAnormal_robot16_pros.csv</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>{0.42499999999999993}</t>
+          <t>{0.32500000000000007}</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>FitAnormal_robot17_pros.csv</t>
+          <t>FitAnormal_robot7_pros.csv</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>{0.32500000000000007}</t>
+          <t>{0.42499999999999993}</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>FitAnormal_robot5_pros.csv</t>
+          <t>FitAnormal_robot17_pros.csv</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>{0.42499999999999993}</t>
+          <t>{0.32500000000000007}</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>FitAnormal_robot13_pros.csv</t>
+          <t>FitAnormal_robot5_pros.csv</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>{0.375}</t>
+          <t>{0.42499999999999993}</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>FitAnormal_robot13_pros.csv</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>{0.375}</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>FitAnormal_robot15_pros.csv</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>{0.32500000000000007}</t>
         </is>

</xml_diff>